<commit_message>
Production insert. NO ERRORS!!
</commit_message>
<xml_diff>
--- a/SW Server Scripts/Migration Scripts/MAX_RID-LEMIR PROD.xlsx
+++ b/SW Server Scripts/Migration Scripts/MAX_RID-LEMIR PROD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\solid-waste-migration\SW Server Scripts\Migration Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D175189C-A50A-4392-B4F8-FEFC48A1D1CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A96B8A4-64E9-4112-B077-DF6F1E7BDECC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65CE3A45-0067-4B06-9F41-9E9096B8512A}"/>
+    <workbookView xWindow="33930" yWindow="2370" windowWidth="22665" windowHeight="11385" xr2:uid="{65CE3A45-0067-4B06-9F41-9E9096B8512A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE228960-DED0-4A74-8B4C-38656CA996E0}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>